<commit_message>
updating the unemployment dataset because it was buggy
</commit_message>
<xml_diff>
--- a/raw-data/DOL-unemployment-rawdata/weekly_unemployment_claims.xlsx
+++ b/raw-data/DOL-unemployment-rawdata/weekly_unemployment_claims.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="87">
   <si>
     <t>date</t>
   </si>
@@ -318,16 +318,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -612,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A970" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A948" sqref="A948:XFD948"/>
+    <sheetView tabSelected="1" topLeftCell="A964" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B982" sqref="B982:C983"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2246,8 +2243,8 @@
       <c r="A90" t="s">
         <v>34</v>
       </c>
-      <c r="B90" s="4">
-        <v>43946</v>
+      <c r="B90" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C90">
         <v>16</v>
@@ -2264,8 +2261,8 @@
       <c r="A91" t="s">
         <v>34</v>
       </c>
-      <c r="B91" s="4">
-        <v>43953</v>
+      <c r="B91" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C91">
         <v>17</v>
@@ -2570,8 +2567,8 @@
       <c r="A108" t="s">
         <v>35</v>
       </c>
-      <c r="B108" s="4">
-        <v>43946</v>
+      <c r="B108" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C108">
         <v>16</v>
@@ -2588,8 +2585,8 @@
       <c r="A109" t="s">
         <v>35</v>
       </c>
-      <c r="B109" s="4">
-        <v>43953</v>
+      <c r="B109" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C109">
         <v>17</v>
@@ -2894,8 +2891,8 @@
       <c r="A126" t="s">
         <v>36</v>
       </c>
-      <c r="B126" s="4">
-        <v>43946</v>
+      <c r="B126" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C126">
         <v>16</v>
@@ -2912,8 +2909,8 @@
       <c r="A127" t="s">
         <v>36</v>
       </c>
-      <c r="B127" s="4">
-        <v>43953</v>
+      <c r="B127" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C127">
         <v>17</v>
@@ -3218,8 +3215,8 @@
       <c r="A144" t="s">
         <v>37</v>
       </c>
-      <c r="B144" s="4">
-        <v>43946</v>
+      <c r="B144" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C144">
         <v>16</v>
@@ -3236,8 +3233,8 @@
       <c r="A145" t="s">
         <v>37</v>
       </c>
-      <c r="B145" s="4">
-        <v>43953</v>
+      <c r="B145" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C145">
         <v>17</v>
@@ -3740,8 +3737,8 @@
       <c r="A173" t="s">
         <v>38</v>
       </c>
-      <c r="B173" s="4">
-        <v>43946</v>
+      <c r="B173" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C173">
         <v>16</v>
@@ -3758,8 +3755,8 @@
       <c r="A174" t="s">
         <v>38</v>
       </c>
-      <c r="B174" s="4">
-        <v>43953</v>
+      <c r="B174" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C174">
         <v>17</v>
@@ -4208,8 +4205,8 @@
       <c r="A199" t="s">
         <v>39</v>
       </c>
-      <c r="B199" s="4">
-        <v>43946</v>
+      <c r="B199" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C199">
         <v>16</v>
@@ -4226,8 +4223,8 @@
       <c r="A200" t="s">
         <v>39</v>
       </c>
-      <c r="B200" s="4">
-        <v>43953</v>
+      <c r="B200" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C200">
         <v>17</v>
@@ -4694,8 +4691,8 @@
       <c r="A226" t="s">
         <v>40</v>
       </c>
-      <c r="B226" s="4">
-        <v>43946</v>
+      <c r="B226" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C226">
         <v>16</v>
@@ -4712,8 +4709,8 @@
       <c r="A227" t="s">
         <v>40</v>
       </c>
-      <c r="B227" s="4">
-        <v>43953</v>
+      <c r="B227" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C227">
         <v>17</v>
@@ -5018,8 +5015,8 @@
       <c r="A244" t="s">
         <v>41</v>
       </c>
-      <c r="B244" s="4">
-        <v>43946</v>
+      <c r="B244" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C244">
         <v>16</v>
@@ -5036,8 +5033,8 @@
       <c r="A245" t="s">
         <v>41</v>
       </c>
-      <c r="B245" s="4">
-        <v>43953</v>
+      <c r="B245" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C245">
         <v>17</v>
@@ -5342,8 +5339,8 @@
       <c r="A262" t="s">
         <v>42</v>
       </c>
-      <c r="B262" s="4">
-        <v>43946</v>
+      <c r="B262" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C262">
         <v>16</v>
@@ -5360,8 +5357,8 @@
       <c r="A263" t="s">
         <v>42</v>
       </c>
-      <c r="B263" s="4">
-        <v>43953</v>
+      <c r="B263" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C263">
         <v>17</v>
@@ -5666,8 +5663,8 @@
       <c r="A280" t="s">
         <v>43</v>
       </c>
-      <c r="B280" s="4">
-        <v>43946</v>
+      <c r="B280" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C280">
         <v>16</v>
@@ -5684,8 +5681,8 @@
       <c r="A281" t="s">
         <v>43</v>
       </c>
-      <c r="B281" s="4">
-        <v>43953</v>
+      <c r="B281" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C281">
         <v>17</v>
@@ -5990,8 +5987,8 @@
       <c r="A298" t="s">
         <v>44</v>
       </c>
-      <c r="B298" s="4">
-        <v>43946</v>
+      <c r="B298" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C298">
         <v>16</v>
@@ -6008,8 +6005,8 @@
       <c r="A299" t="s">
         <v>44</v>
       </c>
-      <c r="B299" s="4">
-        <v>43953</v>
+      <c r="B299" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C299">
         <v>17</v>
@@ -6314,8 +6311,8 @@
       <c r="A316" t="s">
         <v>45</v>
       </c>
-      <c r="B316" s="4">
-        <v>43946</v>
+      <c r="B316" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C316">
         <v>16</v>
@@ -6332,8 +6329,8 @@
       <c r="A317" t="s">
         <v>45</v>
       </c>
-      <c r="B317" s="4">
-        <v>43953</v>
+      <c r="B317" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C317">
         <v>17</v>
@@ -6638,8 +6635,8 @@
       <c r="A334" t="s">
         <v>46</v>
       </c>
-      <c r="B334" s="4">
-        <v>43946</v>
+      <c r="B334" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C334">
         <v>16</v>
@@ -6656,8 +6653,8 @@
       <c r="A335" t="s">
         <v>46</v>
       </c>
-      <c r="B335" s="4">
-        <v>43953</v>
+      <c r="B335" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C335">
         <v>17</v>
@@ -6962,8 +6959,8 @@
       <c r="A352" t="s">
         <v>47</v>
       </c>
-      <c r="B352" s="4">
-        <v>43946</v>
+      <c r="B352" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C352">
         <v>16</v>
@@ -6980,8 +6977,8 @@
       <c r="A353" t="s">
         <v>47</v>
       </c>
-      <c r="B353" s="4">
-        <v>43953</v>
+      <c r="B353" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C353">
         <v>17</v>
@@ -7286,8 +7283,8 @@
       <c r="A370" t="s">
         <v>48</v>
       </c>
-      <c r="B370" s="4">
-        <v>43946</v>
+      <c r="B370" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C370">
         <v>16</v>
@@ -7304,8 +7301,8 @@
       <c r="A371" t="s">
         <v>48</v>
       </c>
-      <c r="B371" s="4">
-        <v>43953</v>
+      <c r="B371" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C371">
         <v>17</v>
@@ -7610,8 +7607,8 @@
       <c r="A388" t="s">
         <v>49</v>
       </c>
-      <c r="B388" s="4">
-        <v>43946</v>
+      <c r="B388" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C388">
         <v>16</v>
@@ -7628,8 +7625,8 @@
       <c r="A389" t="s">
         <v>49</v>
       </c>
-      <c r="B389" s="4">
-        <v>43953</v>
+      <c r="B389" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C389">
         <v>17</v>
@@ -7934,8 +7931,8 @@
       <c r="A406" t="s">
         <v>50</v>
       </c>
-      <c r="B406" s="4">
-        <v>43946</v>
+      <c r="B406" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C406">
         <v>16</v>
@@ -7952,8 +7949,8 @@
       <c r="A407" t="s">
         <v>50</v>
       </c>
-      <c r="B407" s="4">
-        <v>43953</v>
+      <c r="B407" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C407">
         <v>17</v>
@@ -8258,8 +8255,8 @@
       <c r="A424" t="s">
         <v>51</v>
       </c>
-      <c r="B424" s="4">
-        <v>43946</v>
+      <c r="B424" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C424">
         <v>16</v>
@@ -8276,8 +8273,8 @@
       <c r="A425" t="s">
         <v>51</v>
       </c>
-      <c r="B425" s="4">
-        <v>43953</v>
+      <c r="B425" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C425">
         <v>17</v>
@@ -8582,8 +8579,8 @@
       <c r="A442" t="s">
         <v>52</v>
       </c>
-      <c r="B442" s="4">
-        <v>43946</v>
+      <c r="B442" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C442">
         <v>16</v>
@@ -8600,8 +8597,8 @@
       <c r="A443" t="s">
         <v>52</v>
       </c>
-      <c r="B443" s="4">
-        <v>43953</v>
+      <c r="B443" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C443">
         <v>17</v>
@@ -8906,8 +8903,8 @@
       <c r="A460" t="s">
         <v>53</v>
       </c>
-      <c r="B460" s="4">
-        <v>43946</v>
+      <c r="B460" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C460">
         <v>16</v>
@@ -8924,8 +8921,8 @@
       <c r="A461" t="s">
         <v>53</v>
       </c>
-      <c r="B461" s="4">
-        <v>43953</v>
+      <c r="B461" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C461">
         <v>17</v>
@@ -9230,8 +9227,8 @@
       <c r="A478" t="s">
         <v>54</v>
       </c>
-      <c r="B478" s="4">
-        <v>43946</v>
+      <c r="B478" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C478">
         <v>16</v>
@@ -9248,8 +9245,8 @@
       <c r="A479" t="s">
         <v>54</v>
       </c>
-      <c r="B479" s="4">
-        <v>43953</v>
+      <c r="B479" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C479">
         <v>17</v>
@@ -9554,8 +9551,8 @@
       <c r="A496" t="s">
         <v>55</v>
       </c>
-      <c r="B496" s="4">
-        <v>43946</v>
+      <c r="B496" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C496">
         <v>16</v>
@@ -9572,8 +9569,8 @@
       <c r="A497" t="s">
         <v>55</v>
       </c>
-      <c r="B497" s="4">
-        <v>43953</v>
+      <c r="B497" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C497">
         <v>17</v>
@@ -9878,8 +9875,8 @@
       <c r="A514" t="s">
         <v>56</v>
       </c>
-      <c r="B514" s="4">
-        <v>43946</v>
+      <c r="B514" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C514">
         <v>16</v>
@@ -9896,8 +9893,8 @@
       <c r="A515" t="s">
         <v>56</v>
       </c>
-      <c r="B515" s="4">
-        <v>43953</v>
+      <c r="B515" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C515">
         <v>17</v>
@@ -10202,8 +10199,8 @@
       <c r="A532" t="s">
         <v>57</v>
       </c>
-      <c r="B532" s="4">
-        <v>43946</v>
+      <c r="B532" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C532">
         <v>16</v>
@@ -10220,8 +10217,8 @@
       <c r="A533" t="s">
         <v>57</v>
       </c>
-      <c r="B533" s="4">
-        <v>43953</v>
+      <c r="B533" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C533">
         <v>17</v>
@@ -10526,8 +10523,8 @@
       <c r="A550" t="s">
         <v>58</v>
       </c>
-      <c r="B550" s="4">
-        <v>43946</v>
+      <c r="B550" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C550">
         <v>16</v>
@@ -10544,8 +10541,8 @@
       <c r="A551" t="s">
         <v>58</v>
       </c>
-      <c r="B551" s="4">
-        <v>43953</v>
+      <c r="B551" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C551">
         <v>17</v>
@@ -10850,8 +10847,8 @@
       <c r="A568" t="s">
         <v>59</v>
       </c>
-      <c r="B568" s="4">
-        <v>43946</v>
+      <c r="B568" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C568">
         <v>16</v>
@@ -10868,8 +10865,8 @@
       <c r="A569" t="s">
         <v>59</v>
       </c>
-      <c r="B569" s="4">
-        <v>43953</v>
+      <c r="B569" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C569">
         <v>17</v>
@@ -11174,8 +11171,8 @@
       <c r="A586" t="s">
         <v>60</v>
       </c>
-      <c r="B586" s="4">
-        <v>43946</v>
+      <c r="B586" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C586">
         <v>16</v>
@@ -11192,8 +11189,8 @@
       <c r="A587" t="s">
         <v>60</v>
       </c>
-      <c r="B587" s="4">
-        <v>43953</v>
+      <c r="B587" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C587">
         <v>17</v>
@@ -11498,8 +11495,8 @@
       <c r="A604" t="s">
         <v>61</v>
       </c>
-      <c r="B604" s="4">
-        <v>43946</v>
+      <c r="B604" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C604">
         <v>16</v>
@@ -11516,8 +11513,8 @@
       <c r="A605" t="s">
         <v>61</v>
       </c>
-      <c r="B605" s="4">
-        <v>43953</v>
+      <c r="B605" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C605">
         <v>17</v>
@@ -11822,8 +11819,8 @@
       <c r="A622" t="s">
         <v>62</v>
       </c>
-      <c r="B622" s="4">
-        <v>43946</v>
+      <c r="B622" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C622">
         <v>16</v>
@@ -11840,8 +11837,8 @@
       <c r="A623" t="s">
         <v>62</v>
       </c>
-      <c r="B623" s="4">
-        <v>43953</v>
+      <c r="B623" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C623">
         <v>17</v>
@@ -12146,8 +12143,8 @@
       <c r="A640" t="s">
         <v>63</v>
       </c>
-      <c r="B640" s="4">
-        <v>43946</v>
+      <c r="B640" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C640">
         <v>16</v>
@@ -12164,8 +12161,8 @@
       <c r="A641" t="s">
         <v>63</v>
       </c>
-      <c r="B641" s="4">
-        <v>43953</v>
+      <c r="B641" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C641">
         <v>17</v>
@@ -12470,8 +12467,8 @@
       <c r="A658" t="s">
         <v>64</v>
       </c>
-      <c r="B658" s="4">
-        <v>43946</v>
+      <c r="B658" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C658">
         <v>16</v>
@@ -12488,8 +12485,8 @@
       <c r="A659" t="s">
         <v>64</v>
       </c>
-      <c r="B659" s="4">
-        <v>43953</v>
+      <c r="B659" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C659">
         <v>17</v>
@@ -12794,8 +12791,8 @@
       <c r="A676" t="s">
         <v>65</v>
       </c>
-      <c r="B676" s="4">
-        <v>43946</v>
+      <c r="B676" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C676">
         <v>16</v>
@@ -12812,8 +12809,8 @@
       <c r="A677" t="s">
         <v>65</v>
       </c>
-      <c r="B677" s="4">
-        <v>43953</v>
+      <c r="B677" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C677">
         <v>17</v>
@@ -13118,8 +13115,8 @@
       <c r="A694" t="s">
         <v>66</v>
       </c>
-      <c r="B694" s="4">
-        <v>43946</v>
+      <c r="B694" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C694">
         <v>16</v>
@@ -13136,8 +13133,8 @@
       <c r="A695" t="s">
         <v>66</v>
       </c>
-      <c r="B695" s="4">
-        <v>43953</v>
+      <c r="B695" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C695">
         <v>17</v>
@@ -13442,8 +13439,8 @@
       <c r="A712" t="s">
         <v>67</v>
       </c>
-      <c r="B712" s="4">
-        <v>43946</v>
+      <c r="B712" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C712">
         <v>16</v>
@@ -13460,8 +13457,8 @@
       <c r="A713" t="s">
         <v>67</v>
       </c>
-      <c r="B713" s="4">
-        <v>43953</v>
+      <c r="B713" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C713">
         <v>17</v>
@@ -13766,8 +13763,8 @@
       <c r="A730" t="s">
         <v>68</v>
       </c>
-      <c r="B730" s="4">
-        <v>43946</v>
+      <c r="B730" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C730">
         <v>16</v>
@@ -13784,8 +13781,8 @@
       <c r="A731" t="s">
         <v>68</v>
       </c>
-      <c r="B731" s="4">
-        <v>43953</v>
+      <c r="B731" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C731">
         <v>17</v>
@@ -14090,8 +14087,8 @@
       <c r="A748" t="s">
         <v>69</v>
       </c>
-      <c r="B748" s="4">
-        <v>43946</v>
+      <c r="B748" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C748">
         <v>16</v>
@@ -14108,8 +14105,8 @@
       <c r="A749" t="s">
         <v>69</v>
       </c>
-      <c r="B749" s="4">
-        <v>43953</v>
+      <c r="B749" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C749">
         <v>17</v>
@@ -14414,8 +14411,8 @@
       <c r="A766" t="s">
         <v>70</v>
       </c>
-      <c r="B766" s="4">
-        <v>43946</v>
+      <c r="B766" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C766">
         <v>16</v>
@@ -14432,8 +14429,8 @@
       <c r="A767" t="s">
         <v>70</v>
       </c>
-      <c r="B767" s="4">
-        <v>43953</v>
+      <c r="B767" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C767">
         <v>17</v>
@@ -14738,8 +14735,8 @@
       <c r="A784" t="s">
         <v>71</v>
       </c>
-      <c r="B784" s="4">
-        <v>43946</v>
+      <c r="B784" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C784">
         <v>16</v>
@@ -14756,8 +14753,8 @@
       <c r="A785" t="s">
         <v>71</v>
       </c>
-      <c r="B785" s="4">
-        <v>43953</v>
+      <c r="B785" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C785">
         <v>17</v>
@@ -15062,8 +15059,8 @@
       <c r="A802" t="s">
         <v>72</v>
       </c>
-      <c r="B802" s="4">
-        <v>43946</v>
+      <c r="B802" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C802">
         <v>16</v>
@@ -15080,8 +15077,8 @@
       <c r="A803" t="s">
         <v>72</v>
       </c>
-      <c r="B803" s="4">
-        <v>43953</v>
+      <c r="B803" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C803">
         <v>17</v>
@@ -15386,8 +15383,8 @@
       <c r="A820" t="s">
         <v>73</v>
       </c>
-      <c r="B820" s="4">
-        <v>43946</v>
+      <c r="B820" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C820">
         <v>16</v>
@@ -15404,8 +15401,8 @@
       <c r="A821" t="s">
         <v>73</v>
       </c>
-      <c r="B821" s="4">
-        <v>43953</v>
+      <c r="B821" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C821">
         <v>17</v>
@@ -15710,8 +15707,8 @@
       <c r="A838" t="s">
         <v>74</v>
       </c>
-      <c r="B838" s="4">
-        <v>43946</v>
+      <c r="B838" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C838">
         <v>16</v>
@@ -15728,8 +15725,8 @@
       <c r="A839" t="s">
         <v>74</v>
       </c>
-      <c r="B839" s="4">
-        <v>43953</v>
+      <c r="B839" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C839">
         <v>17</v>
@@ -16034,8 +16031,8 @@
       <c r="A856" t="s">
         <v>75</v>
       </c>
-      <c r="B856" s="4">
-        <v>43946</v>
+      <c r="B856" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C856">
         <v>16</v>
@@ -16052,8 +16049,8 @@
       <c r="A857" t="s">
         <v>75</v>
       </c>
-      <c r="B857" s="4">
-        <v>43953</v>
+      <c r="B857" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C857">
         <v>17</v>
@@ -16358,8 +16355,8 @@
       <c r="A874" t="s">
         <v>76</v>
       </c>
-      <c r="B874" s="4">
-        <v>43946</v>
+      <c r="B874" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C874">
         <v>16</v>
@@ -16376,8 +16373,8 @@
       <c r="A875" t="s">
         <v>76</v>
       </c>
-      <c r="B875" s="4">
-        <v>43953</v>
+      <c r="B875" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C875">
         <v>17</v>
@@ -16682,8 +16679,8 @@
       <c r="A892" t="s">
         <v>77</v>
       </c>
-      <c r="B892" s="4">
-        <v>43946</v>
+      <c r="B892" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C892">
         <v>16</v>
@@ -16700,8 +16697,8 @@
       <c r="A893" t="s">
         <v>77</v>
       </c>
-      <c r="B893" s="4">
-        <v>43953</v>
+      <c r="B893" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C893">
         <v>17</v>
@@ -17006,8 +17003,8 @@
       <c r="A910" t="s">
         <v>78</v>
       </c>
-      <c r="B910" s="4">
-        <v>43946</v>
+      <c r="B910" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C910">
         <v>16</v>
@@ -17024,8 +17021,8 @@
       <c r="A911" t="s">
         <v>78</v>
       </c>
-      <c r="B911" s="4">
-        <v>43953</v>
+      <c r="B911" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C911">
         <v>17</v>
@@ -17330,8 +17327,8 @@
       <c r="A928" t="s">
         <v>79</v>
       </c>
-      <c r="B928" s="4">
-        <v>43946</v>
+      <c r="B928" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C928">
         <v>16</v>
@@ -17348,8 +17345,8 @@
       <c r="A929" t="s">
         <v>79</v>
       </c>
-      <c r="B929" s="4">
-        <v>43953</v>
+      <c r="B929" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C929">
         <v>17</v>
@@ -17654,8 +17651,8 @@
       <c r="A946" t="s">
         <v>80</v>
       </c>
-      <c r="B946" s="4">
-        <v>43946</v>
+      <c r="B946" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C946">
         <v>16</v>
@@ -17672,8 +17669,8 @@
       <c r="A947" t="s">
         <v>80</v>
       </c>
-      <c r="B947" s="4">
-        <v>43953</v>
+      <c r="B947" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C947">
         <v>17</v>
@@ -17978,8 +17975,8 @@
       <c r="A964" t="s">
         <v>81</v>
       </c>
-      <c r="B964" s="4">
-        <v>43946</v>
+      <c r="B964" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C964">
         <v>16</v>
@@ -17996,8 +17993,8 @@
       <c r="A965" t="s">
         <v>81</v>
       </c>
-      <c r="B965" s="4">
-        <v>43953</v>
+      <c r="B965" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C965">
         <v>17</v>
@@ -18302,8 +18299,8 @@
       <c r="A982" t="s">
         <v>82</v>
       </c>
-      <c r="B982" s="4">
-        <v>43946</v>
+      <c r="B982" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C982">
         <v>16</v>
@@ -18316,8 +18313,8 @@
       <c r="A983" t="s">
         <v>82</v>
       </c>
-      <c r="B983" s="4">
-        <v>43953</v>
+      <c r="B983" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C983">
         <v>17</v>

</xml_diff>